<commit_message>
minijob-rv beitrag, minor fix in vorsorgeaufwendungen
Former-commit-id: 7d0237eea7822a0690fc9262d44b7d51fee3d70e
</commit_message>
<xml_diff>
--- a/tests/test_data/test_dfs_ssc.xlsx
+++ b/tests/test_data/test_dfs_ssc.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="ssc1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -416,8 +416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,14 +516,15 @@
       </c>
       <c r="L2" s="2">
         <f>R2+S2+T2+U2</f>
-        <v>0</v>
+        <v>10.799999999999999</v>
       </c>
       <c r="Q2">
         <f>0.7547*450+(((850/(850-450))-(450/(850-450)*0.7547))*(C2-450))</f>
         <v>148.22062500000001</v>
       </c>
       <c r="R2">
-        <v>0</v>
+        <f>0.036*C2</f>
+        <v>10.799999999999999</v>
       </c>
       <c r="S2">
         <v>0</v>

</xml_diff>